<commit_message>
al contourmaps inerpolated values,only not from area 2
- something went wrong with the clusteranalysis of area. think that it can maybe be caused because not all RAM was used for this area
-made a smaller rid for this area too
</commit_message>
<xml_diff>
--- a/_RESULTS/Error_budget/error_budget_area2.xlsx
+++ b/_RESULTS/Error_budget/error_budget_area2.xlsx
@@ -414,7 +414,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4806733659468704</v>
+        <v>0.4812034625204658</v>
       </c>
       <c r="E2" t="n">
         <v>3.728306393057234</v>
@@ -438,7 +438,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7652061428218204</v>
+        <v>0.7659577754940337</v>
       </c>
       <c r="E3" t="n">
         <v>3.605889614447373</v>

</xml_diff>